<commit_message>
modified DOI URL and mended the JS for copy to clipboard
</commit_message>
<xml_diff>
--- a/metadata/wrn20/RN20YLD/01-wrn20yield.xlsx
+++ b/metadata/wrn20/RN20YLD/01-wrn20yield.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E0B6A6-58FE-4C0A-B375-566117FC898C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BCEE6B-6FDF-4B3E-B23E-B973936FD031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="945" windowWidth="21600" windowHeight="11385" xr2:uid="{E5D2D046-59C1-4B48-AE90-BA2342879B2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5D2D046-59C1-4B48-AE90-BA2342879B2E}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -4623,10 +4623,10 @@
   <dimension ref="A1:AW122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Q19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:AU1"/>
+      <selection pane="bottomRight" activeCell="AD50" sqref="AD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4850,7 +4850,7 @@
         <v>237</v>
       </c>
       <c r="L2" s="45">
-        <v>35920</v>
+        <v>32268</v>
       </c>
       <c r="M2" s="7">
         <v>117</v>
@@ -4881,10 +4881,10 @@
         <v>0</v>
       </c>
       <c r="AD2" s="45">
-        <v>35884</v>
+        <v>32232</v>
       </c>
       <c r="AE2" s="45">
-        <v>36024</v>
+        <v>32372</v>
       </c>
       <c r="AF2" s="3">
         <v>5.25</v>
@@ -4938,7 +4938,7 @@
         <v>237</v>
       </c>
       <c r="L3" s="45">
-        <v>35920</v>
+        <v>32268</v>
       </c>
       <c r="M3" s="7">
         <v>117</v>
@@ -4969,10 +4969,10 @@
         <v>0</v>
       </c>
       <c r="AD3" s="45">
-        <v>35884</v>
+        <v>32232</v>
       </c>
       <c r="AE3" s="45">
-        <v>36024</v>
+        <v>32372</v>
       </c>
       <c r="AF3" s="3">
         <v>5.61</v>
@@ -5026,7 +5026,7 @@
         <v>237</v>
       </c>
       <c r="L4" s="45">
-        <v>35920</v>
+        <v>32268</v>
       </c>
       <c r="M4" s="7">
         <v>117</v>
@@ -5057,10 +5057,10 @@
         <v>0</v>
       </c>
       <c r="AD4" s="45">
-        <v>35884</v>
+        <v>32232</v>
       </c>
       <c r="AE4" s="45">
-        <v>36024</v>
+        <v>32372</v>
       </c>
       <c r="AF4" s="3">
         <v>5.38</v>
@@ -5114,7 +5114,7 @@
         <v>237</v>
       </c>
       <c r="L5" s="45">
-        <v>35920</v>
+        <v>32268</v>
       </c>
       <c r="M5" s="7">
         <v>117</v>
@@ -5145,10 +5145,10 @@
         <v>0</v>
       </c>
       <c r="AD5" s="45">
-        <v>35884</v>
+        <v>32232</v>
       </c>
       <c r="AE5" s="45">
-        <v>36024</v>
+        <v>32372</v>
       </c>
       <c r="AF5" s="3">
         <v>4.62</v>
@@ -5202,7 +5202,7 @@
         <v>237</v>
       </c>
       <c r="L6" s="45">
-        <v>35920</v>
+        <v>32268</v>
       </c>
       <c r="M6" s="7">
         <v>117</v>
@@ -5233,10 +5233,10 @@
         <v>0</v>
       </c>
       <c r="AD6" s="45">
-        <v>35884</v>
+        <v>32232</v>
       </c>
       <c r="AE6" s="45">
-        <v>36024</v>
+        <v>32372</v>
       </c>
       <c r="AF6" s="3">
         <v>5.44</v>
@@ -5290,7 +5290,7 @@
         <v>237</v>
       </c>
       <c r="L7" s="45">
-        <v>35920</v>
+        <v>32268</v>
       </c>
       <c r="M7" s="7">
         <v>117</v>
@@ -5321,10 +5321,10 @@
         <v>0</v>
       </c>
       <c r="AD7" s="45">
-        <v>35884</v>
+        <v>32232</v>
       </c>
       <c r="AE7" s="45">
-        <v>36024</v>
+        <v>32372</v>
       </c>
       <c r="AF7" s="3">
         <v>5.0999999999999996</v>
@@ -5378,7 +5378,7 @@
         <v>237</v>
       </c>
       <c r="L8" s="45">
-        <v>35920</v>
+        <v>32268</v>
       </c>
       <c r="M8" s="7">
         <v>117</v>
@@ -5409,10 +5409,10 @@
         <v>0</v>
       </c>
       <c r="AD8" s="45">
-        <v>35884</v>
+        <v>32232</v>
       </c>
       <c r="AE8" s="45">
-        <v>36024</v>
+        <v>32372</v>
       </c>
       <c r="AF8" s="3">
         <v>4.62</v>
@@ -5466,7 +5466,7 @@
         <v>237</v>
       </c>
       <c r="L9" s="45">
-        <v>35920</v>
+        <v>32268</v>
       </c>
       <c r="M9" s="7">
         <v>117</v>
@@ -5497,10 +5497,10 @@
         <v>0</v>
       </c>
       <c r="AD9" s="45">
-        <v>35884</v>
+        <v>32232</v>
       </c>
       <c r="AE9" s="45">
-        <v>36024</v>
+        <v>32372</v>
       </c>
       <c r="AF9" s="3">
         <v>5.1100000000000003</v>
@@ -14832,17 +14832,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="bf3d09fe-6738-443d-9673-b7ff0d7dd09c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6584b4ba-af75-4ac8-8379-7172592f8823">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100622C72A1DD75CA4D87E39FE37B04C3D3" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99b455209db282e8e6e2ab1198281278">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6584b4ba-af75-4ac8-8379-7172592f8823" xmlns:ns3="a9e4a452-7199-439f-b4c2-3c6fe4528eb3" xmlns:ns4="bf3d09fe-6738-443d-9673-b7ff0d7dd09c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e79ca979dda8c4f50da160955269f501" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6584b4ba-af75-4ac8-8379-7172592f8823"/>
@@ -15102,7 +15091,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -15111,25 +15100,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0F173A7-CF9B-47F2-B902-E6566A5428C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6584b4ba-af75-4ac8-8379-7172592f8823"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="bf3d09fe-6738-443d-9673-b7ff0d7dd09c"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="a9e4a452-7199-439f-b4c2-3c6fe4528eb3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="bf3d09fe-6738-443d-9673-b7ff0d7dd09c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6584b4ba-af75-4ac8-8379-7172592f8823">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0B8E919-8AA9-49F4-BCE2-9D62FC6B775B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15149,10 +15131,28 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03E22043-EAE0-4057-B37C-A6481D01107B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0F173A7-CF9B-47F2-B902-E6566A5428C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6584b4ba-af75-4ac8-8379-7172592f8823"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bf3d09fe-6738-443d-9673-b7ff0d7dd09c"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="a9e4a452-7199-439f-b4c2-3c6fe4528eb3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>